<commit_message>
traitements retours review NS 0316286aa127a28d8fa778a5784ad587acada5c1
</commit_message>
<xml_diff>
--- a/ig/profiling_researchstudy/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/profiling_researchstudy/StructureDefinition-eclaire-researchstudy.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$72</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -54,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-05T09:33:26+00:00</t>
+    <t>2023-07-05T09:53:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1547,6 +1550,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1728,7 +1746,7 @@
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="6" max="6" width="2.2109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.2109375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="2.1640625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="2.1640625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="95.63671875" customWidth="true" bestFit="true"/>
@@ -1880,7 +1898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>45</v>
       </c>
@@ -1893,7 +1911,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s" s="2">
         <v>46</v>
@@ -1997,7 +2015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>53</v>
       </c>
@@ -2112,7 +2130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>61</v>
       </c>
@@ -2229,7 +2247,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>68</v>
       </c>
@@ -2346,7 +2364,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>77</v>
       </c>
@@ -2463,7 +2481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>85</v>
       </c>
@@ -2580,7 +2598,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>92</v>
       </c>
@@ -2697,7 +2715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>103</v>
       </c>
@@ -2814,7 +2832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>108</v>
       </c>
@@ -2931,7 +2949,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>113</v>
       </c>
@@ -3048,7 +3066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>118</v>
       </c>
@@ -3165,7 +3183,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>123</v>
       </c>
@@ -3282,7 +3300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>128</v>
       </c>
@@ -3401,7 +3419,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>133</v>
       </c>
@@ -3518,7 +3536,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>145</v>
       </c>
@@ -3539,7 +3557,7 @@
         <v>46</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>37</v>
@@ -3637,7 +3655,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>148</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>154</v>
       </c>
@@ -3869,7 +3887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>158</v>
       </c>
@@ -3988,7 +4006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>170</v>
       </c>
@@ -4107,7 +4125,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>182</v>
       </c>
@@ -4226,7 +4244,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>192</v>
       </c>
@@ -4343,7 +4361,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>201</v>
       </c>
@@ -4460,7 +4478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>211</v>
       </c>
@@ -4577,7 +4595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>221</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>36</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>37</v>
@@ -4696,7 +4714,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>224</v>
       </c>
@@ -4811,7 +4829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>225</v>
       </c>
@@ -4928,7 +4946,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>226</v>
       </c>
@@ -5047,7 +5065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
         <v>228</v>
       </c>
@@ -5166,7 +5184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
         <v>229</v>
       </c>
@@ -5285,7 +5303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
         <v>230</v>
       </c>
@@ -5402,7 +5420,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
         <v>231</v>
       </c>
@@ -5519,7 +5537,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
         <v>232</v>
       </c>
@@ -5636,7 +5654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
         <v>233</v>
       </c>
@@ -5753,7 +5771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
         <v>239</v>
       </c>
@@ -5870,7 +5888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
         <v>247</v>
       </c>
@@ -5989,7 +6007,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
         <v>255</v>
       </c>
@@ -6106,7 +6124,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
         <v>263</v>
       </c>
@@ -6223,7 +6241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
         <v>272</v>
       </c>
@@ -6340,7 +6358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
         <v>280</v>
       </c>
@@ -6457,7 +6475,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>286</v>
       </c>
@@ -6574,7 +6592,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
         <v>293</v>
       </c>
@@ -6691,7 +6709,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
         <v>300</v>
       </c>
@@ -6806,7 +6824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
         <v>306</v>
       </c>
@@ -6921,7 +6939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
         <v>307</v>
       </c>
@@ -7038,7 +7056,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
         <v>308</v>
       </c>
@@ -7155,7 +7173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
         <v>313</v>
       </c>
@@ -7272,7 +7290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
         <v>318</v>
       </c>
@@ -7387,7 +7405,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
         <v>326</v>
       </c>
@@ -7504,7 +7522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
         <v>333</v>
       </c>
@@ -7621,7 +7639,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
         <v>339</v>
       </c>
@@ -7738,7 +7756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
         <v>345</v>
       </c>
@@ -7855,7 +7873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
         <v>352</v>
       </c>
@@ -7972,7 +7990,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
         <v>362</v>
       </c>
@@ -8089,7 +8107,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
         <v>371</v>
       </c>
@@ -8206,7 +8224,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
         <v>378</v>
       </c>
@@ -8323,7 +8341,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
         <v>385</v>
       </c>
@@ -8440,7 +8458,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
         <v>392</v>
       </c>
@@ -8557,7 +8575,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
         <v>400</v>
       </c>
@@ -8674,7 +8692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
         <v>407</v>
       </c>
@@ -8789,7 +8807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
         <v>413</v>
       </c>
@@ -8904,7 +8922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
         <v>414</v>
       </c>
@@ -9021,7 +9039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
         <v>415</v>
       </c>
@@ -9140,7 +9158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
         <v>420</v>
       </c>
@@ -9257,7 +9275,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
         <v>425</v>
       </c>
@@ -9374,7 +9392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
         <v>430</v>
       </c>
@@ -9491,7 +9509,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
         <v>435</v>
       </c>
@@ -9606,7 +9624,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
         <v>439</v>
       </c>
@@ -9721,7 +9739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
         <v>440</v>
       </c>
@@ -9838,7 +9856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
         <v>441</v>
       </c>
@@ -9957,7 +9975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
         <v>442</v>
       </c>
@@ -10074,7 +10092,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
         <v>446</v>
       </c>
@@ -10192,6 +10210,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AO72">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI71">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>